<commit_message>
end of level wip
</commit_message>
<xml_diff>
--- a/assets/translation/translations.xlsx
+++ b/assets/translation/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="287">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -427,18 +427,14 @@
   </si>
   <si>
     <t xml:space="preserve">I created all the other assets you'll find in this project. This means:
-- The crappy music playing in the background near the merchant
-- The image of merchant
-- The images used to texture the test level
+- All images used to texture the supermarket
 - All 3D models
 - All sounds (mostly made with https://sfxr.me)
 Feel free to do whatever you want with these and this project.</t>
   </si>
   <si>
     <t xml:space="preserve">J'ai créé toutes les autres ressources de ce projet. À savoir:
-- La musique naze qui joue près du marchand
-- La texture du marchand
-- Les images qui servent à texturer le niveau test
+- Les images qui servent à texturer le supermarché
 - Tous les modèles 3D
 - Tous les sons (principalement générés sur ce site https://sfxr.me)
 N'hésitez pas à faire ce que vous voulez avec ces ressources et le projet lui-même.</t>
@@ -675,15 +671,6 @@
     <t xml:space="preserve">Effets</t>
   </si>
   <si>
-    <t xml:space="preserve">gamma_hint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Increase or lower the gamma value\nGodot's robot must be barely visible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Augmenter ou diminuer le gamma\nle robot de Godot doit être à peine visible</t>
-  </si>
-  <si>
     <t xml:space="preserve">move_forward</t>
   </si>
   <si>
@@ -799,6 +786,111 @@
   </si>
   <si>
     <t xml:space="preserve">"Utiliser" pour démarrer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grocery_list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grocery list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liste de course</t>
+  </si>
+  <si>
+    <t xml:space="preserve">can_of_soup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can of soup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soupe en boîte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">box_of_cereal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cereal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Céréal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viande</t>
+  </si>
+  <si>
+    <t xml:space="preserve">soda_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">soda_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toilet_paper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toilet paper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coffee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coffee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Café</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snacks_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Snacks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snacks_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">instant_noodle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instant Noodle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nouilles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fruits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fruits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vegetables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vegetables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Légumes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sugar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sugar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sucre</t>
   </si>
 </sst>
 </file>
@@ -813,6 +905,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -834,6 +927,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -974,13 +1068,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C97"/>
+  <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C97" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C44" activeCellId="0" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="66.18"/>
@@ -1526,7 +1620,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>133</v>
       </c>
@@ -1916,40 +2010,40 @@
         <v>219</v>
       </c>
       <c r="B85" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="C85" s="0" t="s">
         <v>220</v>
-      </c>
-      <c r="C85" s="0" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="C86" s="0" t="s">
         <v>222</v>
-      </c>
-      <c r="B86" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="C86" s="0" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C87" s="0" t="s">
         <v>224</v>
-      </c>
-      <c r="B87" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="C87" s="0" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="B88" s="0" t="s">
         <v>226</v>
-      </c>
-      <c r="B88" s="0" t="s">
-        <v>92</v>
       </c>
       <c r="C88" s="0" t="s">
         <v>227</v>
@@ -2052,6 +2146,149 @@
       </c>
       <c r="C97" s="0" t="s">
         <v>254</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="C98" s="0" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="C99" s="0" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="B100" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="C100" s="0" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="C101" s="0" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="C102" s="0" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="B103" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="C103" s="0" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="B104" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="C104" s="0" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="B105" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="C105" s="0" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="B106" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="C106" s="0" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="B107" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="C107" s="0" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="B108" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="C108" s="0" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="B109" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="C109" s="0" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="B110" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="C110" s="0" t="s">
+        <v>286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>